<commit_message>
added input error handling
</commit_message>
<xml_diff>
--- a/test/input_file/inputparameters.xlsx
+++ b/test/input_file/inputparameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input_variables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
   <si>
     <t>0.3</t>
   </si>
@@ -59,18 +59,12 @@
     <t>f_y</t>
   </si>
   <si>
-    <t>Wheel materials</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>norm</t>
   </si>
   <si>
-    <t>material number</t>
-  </si>
-  <si>
     <t>hardened</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>EN10083-3</t>
   </si>
   <si>
-    <t>Rail materials</t>
-  </si>
-  <si>
     <t>S235</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>"unknown"</t>
   </si>
   <si>
-    <t>add the desired material and its parameteres if it is not among the materials below</t>
-  </si>
-  <si>
     <t>GE-300</t>
   </si>
   <si>
@@ -324,6 +312,9 @@
   </si>
   <si>
     <t>num_cycles</t>
+  </si>
+  <si>
+    <t>material_number</t>
   </si>
 </sst>
 </file>
@@ -334,7 +325,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,22 +364,8 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,11 +386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -499,13 +471,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,26 +512,16 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
     <cellStyle name="Gut" xfId="2" builtinId="26"/>
-    <cellStyle name="Schlecht" xfId="3" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
@@ -810,12 +771,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="railmaterials" displayName="railmaterials" ref="A2:I9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Gut">
-  <autoFilter ref="A2:I9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="railmaterials" displayName="railmaterials" ref="A1:I8" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Gut">
+  <autoFilter ref="A1:I8"/>
   <tableColumns count="9">
     <tableColumn id="1" name="name" dataDxfId="19"/>
     <tableColumn id="2" name="norm" dataDxfId="18"/>
-    <tableColumn id="3" name="material number" dataDxfId="17"/>
+    <tableColumn id="3" name="material_number" dataDxfId="17"/>
     <tableColumn id="4" name="hardened" dataDxfId="16"/>
     <tableColumn id="5" name="f_y" dataDxfId="15"/>
     <tableColumn id="6" name="HB" dataDxfId="14"/>
@@ -828,12 +789,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="wheelmaterials4" displayName="wheelmaterials4" ref="A2:I10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Gut">
-  <autoFilter ref="A2:I10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="wheelmaterials4" displayName="wheelmaterials4" ref="A1:I9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Gut">
+  <autoFilter ref="A1:I9"/>
   <tableColumns count="9">
     <tableColumn id="1" name="name" dataDxfId="8"/>
     <tableColumn id="2" name="norm" dataDxfId="7"/>
-    <tableColumn id="3" name="material number" dataDxfId="6"/>
+    <tableColumn id="3" name="material_number" dataDxfId="6"/>
     <tableColumn id="4" name="hardened" dataDxfId="5"/>
     <tableColumn id="9" name="z" dataDxfId="4"/>
     <tableColumn id="5" name="f_y" dataDxfId="3"/>
@@ -1144,19 +1105,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="4" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1176,7 +1137,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1177,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1236,9 +1197,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3">
         <v>10</v>
@@ -1256,9 +1217,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3">
         <v>10</v>
@@ -1276,9 +1237,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3">
         <v>10</v>
@@ -1296,9 +1257,9 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3">
         <v>2000</v>
@@ -1316,9 +1277,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3">
         <v>5.0000000000000001E-3</v>
@@ -1336,29 +1297,29 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -1376,9 +1337,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -1396,49 +1357,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B15" s="3">
         <v>20000</v>
@@ -1456,9 +1417,9 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B16" s="3">
         <v>20000</v>
@@ -1476,9 +1437,9 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B17" s="3">
         <v>100000</v>
@@ -1512,13 +1473,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="If the desired material does not figrue on the list, please add it as well as its following parameters to the list in the worksheet &quot;rail and wheel materials&quot;">
           <x14:formula1>
-            <xm:f>rail_materials!$A$3:$A$9</xm:f>
+            <xm:f>rail_materials!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C14:F14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note " prompt="If the desired material does not figure on the list, please add it as well as its following parameters manuelly to the list in the worksheet &quot;rail and wheel materials&quot;">
           <x14:formula1>
-            <xm:f>wheel_materials!$A$3:$A$10</xm:f>
+            <xm:f>wheel_materials!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>C13:V13</xm:sqref>
         </x14:dataValidation>
@@ -1536,17 +1497,17 @@
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1">
         <v>24.9397924881983</v>
@@ -1564,12 +1525,12 @@
         <v>24.603567265875999</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>0.397534327540081</v>
@@ -1587,12 +1548,12 @@
         <v>0.39281645770158102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>310.53423258511901</v>
@@ -1610,12 +1571,12 @@
         <v>217.83710715883799</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>0.43852951083798603</v>
@@ -1633,12 +1594,12 @@
         <v>0.33759378483001701</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>9592.8821295104699</v>
@@ -1656,12 +1617,12 @@
         <v>7039.1850549506698</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>6.9859353305379797</v>
@@ -1679,12 +1640,12 @@
         <v>7.9973902757422897</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>0.36032232455732299</v>
@@ -1702,12 +1663,12 @@
         <v>0.43685550941856799</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>235.360704664796</v>
@@ -1725,12 +1686,12 @@
         <v>391.55736926069602</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>3620.8448324163101</v>
@@ -1748,12 +1709,12 @@
         <v>3659.2272904198899</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>1.13373577673032</v>
@@ -1771,12 +1732,12 @@
         <v>0.99721191005946297</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>0.67575877439752896</v>
@@ -1794,12 +1755,12 @@
         <v>0.74159415955053198</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C12">
         <v>3.8387980542432998</v>
@@ -1817,12 +1778,12 @@
         <v>1.56466211459187</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>0.82317441160238602</v>
@@ -1840,12 +1801,12 @@
         <v>0.58201942471427504</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C14">
         <v>2351.0358557609202</v>
@@ -1863,12 +1824,12 @@
         <v>5316.4232733114604</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C15">
         <v>479.56427978543297</v>
@@ -1886,12 +1847,12 @@
         <v>1431.3338377950799</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C16">
         <v>1.5209241133552001</v>
@@ -1909,12 +1870,12 @@
         <v>0.97421919684422997</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C17">
         <v>148.023377589456</v>
@@ -1939,71 +1900,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>360</v>
+      </c>
+      <c r="F2" s="6">
+        <v>125</v>
+      </c>
+      <c r="G2" s="6">
+        <v>210000</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>360</v>
+        <v>410</v>
       </c>
       <c r="F3" s="6">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="G3" s="6">
         <v>210000</v>
@@ -2015,24 +2000,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>410</v>
+        <v>520</v>
       </c>
       <c r="F4" s="6">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="G4" s="6">
         <v>210000</v>
@@ -2044,24 +2029,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>35</v>
+      <c r="C5" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>520</v>
+        <v>760</v>
       </c>
       <c r="F5" s="6">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="G5" s="6">
         <v>210000</v>
@@ -2073,24 +2058,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
       </c>
       <c r="E6" s="6">
-        <v>760</v>
+        <v>520</v>
       </c>
       <c r="F6" s="6">
-        <v>225</v>
+        <v>155</v>
       </c>
       <c r="G6" s="6">
         <v>210000</v>
@@ -2102,24 +2087,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
       </c>
       <c r="E7" s="6">
-        <v>520</v>
+        <v>640</v>
       </c>
       <c r="F7" s="6">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="G7" s="6">
         <v>210000</v>
@@ -2131,12 +2116,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>31</v>
@@ -2145,10 +2130,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="6">
-        <v>640</v>
+        <v>870</v>
       </c>
       <c r="F8" s="6">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="G8" s="6">
         <v>210000</v>
@@ -2157,35 +2142,6 @@
         <v>0</v>
       </c>
       <c r="I8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>870</v>
-      </c>
-      <c r="F9" s="6">
-        <v>260</v>
-      </c>
-      <c r="G9" s="6">
-        <v>210000</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2201,173 +2157,187 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1.6552</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>520</v>
+      </c>
+      <c r="G2" s="5">
+        <v>155</v>
+      </c>
+      <c r="H2" s="5">
+        <v>210000</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>600</v>
+      </c>
+      <c r="G3" s="10">
+        <v>210</v>
+      </c>
+      <c r="H3" s="5">
+        <v>177000</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>700</v>
+      </c>
+      <c r="G4" s="10">
+        <v>245</v>
+      </c>
+      <c r="H4" s="5">
+        <v>180000</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.7218</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>650</v>
+      </c>
+      <c r="G5" s="10">
+        <v>190</v>
+      </c>
+      <c r="H5" s="5">
+        <v>210000</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12">
-        <v>1.6552</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>520</v>
-      </c>
-      <c r="G3" s="5">
-        <v>155</v>
-      </c>
-      <c r="H3" s="5">
-        <v>210000</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0.70599999999999996</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>600</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="C6" s="11">
+        <v>1.7224999999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>700</v>
+      </c>
+      <c r="G6" s="10">
         <v>210</v>
-      </c>
-      <c r="H4" s="5">
-        <v>177000</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="11">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10">
-        <v>700</v>
-      </c>
-      <c r="G5" s="10">
-        <v>245</v>
-      </c>
-      <c r="H5" s="5">
-        <v>180000</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1.7218</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
-        <v>650</v>
-      </c>
-      <c r="G6" s="10">
-        <v>190</v>
       </c>
       <c r="H6" s="5">
         <v>210000</v>
@@ -2376,12 +2346,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="11">
         <v>1.7224999999999999</v>
@@ -2393,10 +2363,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="10">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="G7" s="10">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="H7" s="5">
         <v>210000</v>
@@ -2405,15 +2375,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11">
-        <v>1.7224999999999999</v>
+        <v>1.6956</v>
       </c>
       <c r="D8" s="5">
         <v>0</v>
@@ -2422,10 +2392,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="10">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="G8" s="10">
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="H8" s="5">
         <v>210000</v>
@@ -2434,27 +2404,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="11">
-        <v>1.6956</v>
+        <v>1.7224999999999999</v>
       </c>
       <c r="D9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="10">
-        <v>1000</v>
+        <v>420</v>
       </c>
       <c r="G9" s="10">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="H9" s="5">
         <v>210000</v>
@@ -2463,39 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1.7224999999999999</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>10</v>
-      </c>
-      <c r="F10" s="10">
-        <v>420</v>
-      </c>
-      <c r="G10" s="10">
-        <v>252</v>
-      </c>
-      <c r="H10" s="5">
-        <v>210000</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>